<commit_message>
Implemented comprehensive finite element method for slope stability analysis
  - Added fem.py with complete FEM framework supporting all required element types
  - Implemented elastic-plastic analysis with Mohr-Coulomb yield criterion
  - Added Shear Strength Reduction Method (SSRM) for factor of safety calculation
  - Supported tri3, tri6, quad4, quad8, quad9 elements with proper shape functions
  - Included numerical integration schemes and stress recovery for all element types
  - Added 1D truss elements for soil reinforcement modeling
  - Created plot_fem.py with comprehensive visualization capabilities
  - Added main_fem.py test suite with synthetic examples and input file integration
  - Implemented proper boundary conditions, plastic corrector algorithms, and convergence
   checking
</commit_message>
<xml_diff>
--- a/inputs/slope/input_template_MASTER6.xlsx
+++ b/inputs/slope/input_template_MASTER6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jones/CursorProjects/xslope/inputs/slope/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/cursor_projects/xslope/inputs/slope/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEA8E6E-A20D-4A49-B903-E295619591BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5183405C-372B-1144-888B-A7172148CF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="29340" windowHeight="17300" activeTab="8" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
+    <workbookView xWindow="25240" yWindow="2700" windowWidth="36380" windowHeight="18420" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
     <definedName name="solution2">mat!$L$21</definedName>
     <definedName name="version">main!$D$5</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,6 +47,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -5146,7 +5147,7 @@
       <xdr:col>16</xdr:col>
       <xdr:colOff>780143</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>163286</xdr:rowOff>
+      <xdr:rowOff>54428</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5162,7 +5163,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9180286" y="498930"/>
-          <a:ext cx="4354286" cy="2857499"/>
+          <a:ext cx="4354286" cy="2748641"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5296,7 +5297,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> = modulus of elasticity of reinforcement material [psi or N/m^2]</a:t>
+            <a:t> = modulus of elasticity of reinforcement material</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -5309,7 +5310,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> = cross-sectional area (per unit width) of reinforcement material [in^2 or m^2]</a:t>
+            <a:t> = cross-sectional area (per unit width) of reinforcement material </a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -5639,8 +5640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02E090B-D957-7046-AD33-44E170F709C1}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5666,7 +5667,7 @@
         <v>82</v>
       </c>
       <c r="D5" s="39">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -6588,16 +6589,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="M4:N4"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="J22:K22"/>
     <mergeCell ref="M22:N22"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="M4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6607,8 +6608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA88A0E-2BF5-FE49-9603-08BE4D91829B}">
   <dimension ref="A1:X28"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6617,6 +6618,7 @@
     <col min="2" max="2" width="17.33203125" style="1" customWidth="1"/>
     <col min="3" max="9" width="8.5" style="1" customWidth="1"/>
     <col min="10" max="13" width="8.5" customWidth="1"/>
+    <col min="23" max="23" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">
@@ -6772,7 +6774,7 @@
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
-      <c r="W4" s="4"/>
+      <c r="W4" s="3"/>
       <c r="X4" s="4"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
@@ -6816,7 +6818,7 @@
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
-      <c r="W5" s="4"/>
+      <c r="W5" s="3"/>
       <c r="X5" s="4"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
@@ -6860,7 +6862,7 @@
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
-      <c r="W6" s="4"/>
+      <c r="W6" s="3"/>
       <c r="X6" s="4"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
@@ -6900,7 +6902,7 @@
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
-      <c r="W7" s="4"/>
+      <c r="W7" s="3"/>
       <c r="X7" s="4"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
@@ -6928,7 +6930,7 @@
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
-      <c r="W8" s="4"/>
+      <c r="W8" s="3"/>
       <c r="X8" s="4"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
@@ -6956,7 +6958,7 @@
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
-      <c r="W9" s="4"/>
+      <c r="W9" s="3"/>
       <c r="X9" s="4"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
@@ -6984,7 +6986,7 @@
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
       <c r="V10" s="3"/>
-      <c r="W10" s="4"/>
+      <c r="W10" s="3"/>
       <c r="X10" s="4"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
@@ -7012,7 +7014,7 @@
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
       <c r="V11" s="3"/>
-      <c r="W11" s="4"/>
+      <c r="W11" s="3"/>
       <c r="X11" s="4"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
@@ -7040,7 +7042,7 @@
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
-      <c r="W12" s="4"/>
+      <c r="W12" s="3"/>
       <c r="X12" s="4"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.2">
@@ -7068,7 +7070,7 @@
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
       <c r="V13" s="3"/>
-      <c r="W13" s="4"/>
+      <c r="W13" s="3"/>
       <c r="X13" s="4"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.2">
@@ -7096,7 +7098,7 @@
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
       <c r="V14" s="3"/>
-      <c r="W14" s="4"/>
+      <c r="W14" s="3"/>
       <c r="X14" s="4"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
@@ -7124,10 +7126,10 @@
       <c r="T15" s="3"/>
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
-      <c r="W15" s="4"/>
+      <c r="W15" s="3"/>
       <c r="X15" s="4"/>
     </row>
-    <row r="18" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>59</v>
       </c>
@@ -7137,8 +7139,9 @@
       <c r="K18" s="6" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="19" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="W18" s="5"/>
+    </row>
+    <row r="19" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C19" s="24" t="s">
         <v>87</v>
       </c>
@@ -7157,7 +7160,7 @@
       <c r="P19" s="44"/>
       <c r="Q19" s="44"/>
     </row>
-    <row r="20" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20"/>
@@ -7174,7 +7177,7 @@
       <c r="P20" s="44"/>
       <c r="Q20" s="44"/>
     </row>
-    <row r="21" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C21" s="6" t="s">
         <v>69</v>
       </c>
@@ -7191,7 +7194,7 @@
       <c r="P21" s="44"/>
       <c r="Q21" s="44"/>
     </row>
-    <row r="22" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C22" s="1" t="s">
         <v>68</v>
       </c>
@@ -7201,7 +7204,7 @@
       <c r="E22"/>
       <c r="F22"/>
     </row>
-    <row r="23" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C23" s="1" t="s">
         <v>71</v>
       </c>
@@ -7211,13 +7214,13 @@
       <c r="E23"/>
       <c r="F23"/>
     </row>
-    <row r="24" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24"/>
     </row>
-    <row r="25" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C25" s="6" t="s">
         <v>101</v>
       </c>
@@ -7225,7 +7228,7 @@
       <c r="E25"/>
       <c r="F25"/>
     </row>
-    <row r="26" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C26" s="1" t="s">
         <v>104</v>
       </c>
@@ -7235,7 +7238,7 @@
       <c r="E26"/>
       <c r="F26"/>
     </row>
-    <row r="27" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C27" s="1" t="s">
         <v>21</v>
       </c>
@@ -7245,7 +7248,7 @@
       <c r="E27"/>
       <c r="F27"/>
     </row>
-    <row r="28" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C28" s="1" t="s">
         <v>105</v>
       </c>
@@ -8346,8 +8349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C4F752-BCE4-AE4E-BC09-D828329F219B}">
   <dimension ref="A2:K25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>